<commit_message>
successful compilation using nvfortran
</commit_message>
<xml_diff>
--- a/docs/CFL3D_Variables.xlsx
+++ b/docs/CFL3D_Variables.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D62453-DDF8-4F6F-8F26-85712C10C10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071298D6-3417-4554-9E9D-9F9FFFEA0BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="12" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="文件号" sheetId="3" r:id="rId1"/>
@@ -2825,10 +2825,6 @@
   </si>
   <si>
     <t>前两个量是位置，第三个量为1或者2表示0或dim，其值为边界条件类型，格心为0或格边为1，见bc.F  261行，在实际操作中会影响重构的表达式（见gfluxr.F 191行，还会影响固壁边界判断）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bcdata(mdim,ndim,2,12)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3724,6 +3720,9 @@
   <si>
     <t>最密网格（iseq=mseq=3），全部三层均用三阶muscl。没用一阶精度</t>
   </si>
+  <si>
+    <t>bcdata(mdim,ndim,2,12)</t>
+  </si>
 </sst>
 </file>
 
@@ -3818,7 +3817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3833,13 +3832,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3863,19 +3859,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4456,10 +4443,10 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="119.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="119.1796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="70" style="3" customWidth="1"/>
     <col min="4" max="16384" width="9" style="3"/>
   </cols>
@@ -4487,18 +4474,18 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="19">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="19">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>218</v>
       </c>
     </row>
@@ -4507,7 +4494,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4677,7 +4664,7 @@
         <v>35</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4701,7 +4688,7 @@
         <v>101</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4709,7 +4696,7 @@
         <v>92</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4725,23 +4712,23 @@
         <v>94</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
         <v>95</v>
       </c>
-      <c r="B35" s="24" t="s">
-        <v>826</v>
+      <c r="B35" s="20" t="s">
+        <v>825</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="21">
+      <c r="A36" s="2">
         <v>96</v>
       </c>
-      <c r="B36" s="22" t="s">
-        <v>831</v>
+      <c r="B36" s="3" t="s">
+        <v>830</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4749,15 +4736,15 @@
         <v>97</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
         <v>98</v>
       </c>
-      <c r="B38" s="24" t="s">
-        <v>821</v>
+      <c r="B38" s="20" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4765,7 +4752,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4797,7 +4784,7 @@
         <v>901</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4808,7 +4795,7 @@
         <v>1011</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4834,7 +4821,7 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -4860,15 +4847,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+    <col min="2" max="2" width="28.90625" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
     <col min="4" max="4" width="129" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4961,7 +4948,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="D10" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5029,17 +5016,17 @@
         <v>444</v>
       </c>
       <c r="D18" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="D19" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="D20" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5080,14 +5067,14 @@
         <v>560</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.8">
+    <row r="28" spans="1:4" ht="29">
       <c r="A28" s="7" t="s">
         <v>588</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="17" t="s">
-        <v>851</v>
+      <c r="D28" s="16" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5141,25 +5128,25 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="104.109375" customWidth="1"/>
+    <col min="4" max="4" width="104.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5175,17 +5162,17 @@
         <v>435</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2">
+    <row r="3" spans="1:4" ht="43.5">
       <c r="A3" s="3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="13" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="57.6">
+      <c r="D3" s="12" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="58">
       <c r="A4" s="3" t="s">
         <v>437</v>
       </c>
@@ -5193,8 +5180,8 @@
         <v>451</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="13" t="s">
-        <v>754</v>
+      <c r="D4" s="12" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5233,7 +5220,7 @@
         <v>677</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5253,47 +5240,47 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>784</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>789</v>
+        <v>783</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="D14" s="27"/>
+        <v>782</v>
+      </c>
+      <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>786</v>
-      </c>
-      <c r="D15" s="27"/>
+        <v>785</v>
+      </c>
+      <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:4">
       <c r="D16" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="D17" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="D18" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="D19" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="D20" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5301,7 +5288,7 @@
         <v>681</v>
       </c>
       <c r="D21" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
   </sheetData>
@@ -5322,12 +5309,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
-    <col min="4" max="4" width="59.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
+    <col min="4" max="4" width="59.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5359,12 +5346,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="82.44140625" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5386,7 +5373,7 @@
         <v>452</v>
       </c>
       <c r="D2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5409,23 +5396,23 @@
       <c r="A5" t="s">
         <v>467</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8">
+    <row r="6" spans="1:4" ht="29">
       <c r="A6" t="s">
         <v>469</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8">
+    <row r="7" spans="1:4" ht="29">
       <c r="A7" t="s">
         <v>470</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>471</v>
       </c>
     </row>
@@ -5441,7 +5428,7 @@
       <c r="A9" t="s">
         <v>474</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>475</v>
       </c>
     </row>
@@ -5457,8 +5444,8 @@
       <c r="A11" t="s">
         <v>479</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>785</v>
+      <c r="D11" s="9" t="s">
+        <v>784</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5497,30 +5484,30 @@
         <v>491</v>
       </c>
       <c r="D17" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C18" t="s">
         <v>605</v>
       </c>
       <c r="D18" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="273.60000000000002">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="275.5">
       <c r="A19" s="3" t="s">
         <v>457</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>864</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>834</v>
+        <v>863</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>833</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5528,7 +5515,7 @@
         <v>606</v>
       </c>
       <c r="D20" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
   </sheetData>
@@ -5546,12 +5533,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" customWidth="1"/>
-    <col min="4" max="4" width="82.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="3" max="3" width="40.1796875" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5568,7 +5555,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2">
+    <row r="2" spans="1:4" ht="43.5">
       <c r="A2" s="3" t="s">
         <v>457</v>
       </c>
@@ -5576,7 +5563,7 @@
       <c r="C2" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>602</v>
       </c>
     </row>
@@ -5603,12 +5590,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="68.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.90625" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
+    <col min="3" max="3" width="23.08984375" customWidth="1"/>
+    <col min="4" max="4" width="68.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5625,41 +5612,41 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8">
+    <row r="2" spans="1:4" ht="29">
       <c r="A2" t="s">
         <v>486</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2">
+    <row r="3" spans="1:4" ht="43.5">
       <c r="A3" t="s">
         <v>578</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>781</v>
+      <c r="D3" s="9" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>779</v>
-      </c>
-      <c r="D4" s="27" t="s">
+        <v>778</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>780</v>
-      </c>
-      <c r="D5" s="27"/>
+        <v>779</v>
+      </c>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>782</v>
-      </c>
-      <c r="D6" s="27"/>
+        <v>781</v>
+      </c>
+      <c r="D6" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5679,12 +5666,12 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="47.109375" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.08984375" customWidth="1"/>
+    <col min="2" max="2" width="35.08984375" customWidth="1"/>
+    <col min="3" max="3" width="33.6328125" customWidth="1"/>
+    <col min="4" max="4" width="39.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5703,68 +5690,68 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>735</v>
+      </c>
+      <c r="B2" t="s">
         <v>736</v>
       </c>
-      <c r="B2" t="s">
-        <v>737</v>
-      </c>
       <c r="D2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>737</v>
+      </c>
+      <c r="B3" t="s">
         <v>738</v>
       </c>
-      <c r="B3" t="s">
-        <v>739</v>
-      </c>
       <c r="D3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>741</v>
+      </c>
+      <c r="B4" t="s">
+        <v>738</v>
+      </c>
+      <c r="D4" t="s">
         <v>742</v>
-      </c>
-      <c r="B4" t="s">
-        <v>739</v>
-      </c>
-      <c r="D4" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>743</v>
+      </c>
+      <c r="B5" t="s">
+        <v>738</v>
+      </c>
+      <c r="D5" t="s">
         <v>744</v>
-      </c>
-      <c r="B5" t="s">
-        <v>739</v>
-      </c>
-      <c r="D5" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>745</v>
+      </c>
+      <c r="B6" t="s">
+        <v>738</v>
+      </c>
+      <c r="D6" t="s">
         <v>746</v>
-      </c>
-      <c r="B6" t="s">
-        <v>739</v>
-      </c>
-      <c r="D6" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>747</v>
+      </c>
+      <c r="B7" t="s">
+        <v>738</v>
+      </c>
+      <c r="D7" t="s">
         <v>748</v>
-      </c>
-      <c r="B7" t="s">
-        <v>739</v>
-      </c>
-      <c r="D7" t="s">
-        <v>749</v>
       </c>
     </row>
   </sheetData>
@@ -5782,12 +5769,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6328125" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" customWidth="1"/>
+    <col min="4" max="4" width="43.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5804,14 +5791,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.8">
+    <row r="2" spans="1:4" ht="29">
       <c r="A2" t="s">
         <v>488</v>
       </c>
       <c r="B2" t="s">
         <v>489</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>490</v>
       </c>
     </row>
@@ -5840,11 +5827,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="4" width="30.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="4" width="30.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5875,25 +5862,25 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="135.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="3" max="3" width="135.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C2" t="s">
         <v>344</v>
@@ -5920,124 +5907,124 @@
         <v>581</v>
       </c>
       <c r="C5" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.5">
       <c r="A6" t="s">
-        <v>825</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>829</v>
+        <v>824</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>828</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C7" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C8" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="9" t="s">
-        <v>815</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9" t="s">
-        <v>835</v>
+      <c r="A9" s="8" t="s">
+        <v>814</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>834</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="23" t="s">
-        <v>801</v>
+      <c r="A10" s="19" t="s">
+        <v>800</v>
       </c>
       <c r="C10" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="19" t="s">
+        <v>805</v>
+      </c>
+      <c r="C11" t="s">
         <v>832</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="23" t="s">
-        <v>806</v>
-      </c>
-      <c r="C11" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>822</v>
+      </c>
+      <c r="C12" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.5">
+      <c r="A13" t="s">
+        <v>821</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>823</v>
-      </c>
-      <c r="C12" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="43.2">
-      <c r="A13" t="s">
-        <v>822</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C14" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C15" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C17" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C18" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -6055,12 +6042,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6088,7 +6075,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="14"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -6103,7 +6090,7 @@
       <c r="C12" s="7" t="s">
         <v>552</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>553</v>
       </c>
     </row>
@@ -6178,7 +6165,7 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -6208,12 +6195,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="3" width="40.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6246,15 +6233,15 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D4" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -6308,30 +6295,30 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D14" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="D15" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="D16" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2">
-      <c r="D17" s="10" t="s">
-        <v>790</v>
+        <v>751</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.5">
+      <c r="D17" s="9" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -6362,15 +6349,15 @@
         <v>708</v>
       </c>
       <c r="D25" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="72">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="72.5">
       <c r="A29" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>768</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>769</v>
       </c>
     </row>
   </sheetData>
@@ -6388,7 +6375,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="4" max="4" width="76" bestFit="1" customWidth="1"/>
   </cols>
@@ -6426,15 +6413,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A2:E90"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" customWidth="1"/>
-    <col min="4" max="4" width="90.5546875" customWidth="1"/>
-    <col min="5" max="5" width="85.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="4" max="4" width="90.54296875" customWidth="1"/>
+    <col min="5" max="5" width="85.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
@@ -6447,92 +6434,92 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>872</v>
+      </c>
+      <c r="D4" t="s">
         <v>711</v>
-      </c>
-      <c r="D4" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D9" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="E11" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="E12" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="E13" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
+        <v>716</v>
+      </c>
+      <c r="E14" t="s">
         <v>717</v>
-      </c>
-      <c r="E14" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>718</v>
+      </c>
+      <c r="E15" t="s">
         <v>719</v>
-      </c>
-      <c r="E15" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>720</v>
+      </c>
+      <c r="E16" t="s">
         <v>721</v>
-      </c>
-      <c r="E16" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="19" spans="5:5" ht="28.8">
-      <c r="E19" s="10" t="s">
-        <v>799</v>
+        <v>723</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" ht="43.5">
+      <c r="E19" s="9" t="s">
+        <v>798</v>
       </c>
     </row>
     <row r="20" spans="5:5">
       <c r="E20" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="44" spans="1:1">
@@ -6542,33 +6529,33 @@
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="16" t="s">
-        <v>730</v>
+      <c r="A82" s="15" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
+        <v>730</v>
+      </c>
+      <c r="D83" t="s">
         <v>731</v>
-      </c>
-      <c r="D83" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
+        <v>732</v>
+      </c>
+      <c r="D84" t="s">
         <v>733</v>
       </c>
-      <c r="D84" t="s">
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="15" t="s">
         <v>734</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="16" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -6603,9 +6590,9 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6686,14 +6673,14 @@
       <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="32.77734375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="81.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="81.453125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="8.6640625" style="7"/>
+    <col min="6" max="16384" width="8.6328125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7073,18 +7060,18 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="7" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="7" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>19</v>
@@ -7093,9 +7080,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.8">
-      <c r="D40" s="18" t="s">
-        <v>805</v>
+    <row r="40" spans="1:4" ht="29">
+      <c r="D40" s="16" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -7576,7 +7563,7 @@
         <v>154</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -7586,8 +7573,8 @@
       <c r="B94" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D94" s="8" t="s">
-        <v>865</v>
+      <c r="D94" s="7" t="s">
+        <v>864</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -7631,7 +7618,7 @@
         <v>165</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -7834,7 +7821,7 @@
         <v>361</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -7845,7 +7832,7 @@
         <v>361</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -7971,10 +7958,10 @@
         <v>357</v>
       </c>
       <c r="B146" s="7" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D146" s="7" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -8212,11 +8199,11 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -8255,15 +8242,15 @@
         <v>305</v>
       </c>
       <c r="D3" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="86.4">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="87">
       <c r="A4" t="s">
         <v>306</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>856</v>
+      <c r="D4" s="9" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8293,7 +8280,7 @@
         <v>314</v>
       </c>
       <c r="D8" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -8359,7 +8346,7 @@
         <v>318</v>
       </c>
       <c r="D21" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -8373,15 +8360,15 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.8">
+    <row r="24" spans="1:4" ht="29">
       <c r="A24" t="s">
         <v>320</v>
       </c>
       <c r="C24" t="s">
         <v>321</v>
       </c>
-      <c r="D24" s="25" t="s">
-        <v>862</v>
+      <c r="D24" s="21" t="s">
+        <v>861</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -8389,7 +8376,7 @@
         <v>332</v>
       </c>
       <c r="D26" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -8404,8 +8391,8 @@
       <c r="A29" t="s">
         <v>391</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>857</v>
+      <c r="D29" s="8" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -8418,19 +8405,19 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
+        <v>866</v>
+      </c>
+      <c r="D31" t="s">
         <v>867</v>
-      </c>
-      <c r="D31" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="D32" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>394</v>
       </c>
     </row>
@@ -8469,12 +8456,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="223.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="223.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -8641,11 +8628,11 @@
         <v>512</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -8876,14 +8863,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="117.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="117.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -9082,7 +9069,7 @@
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -9138,7 +9125,7 @@
         <v>673</v>
       </c>
       <c r="D48" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -9146,12 +9133,12 @@
         <v>674</v>
       </c>
       <c r="D50" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D52" t="s">
         <v>675</v>
@@ -9159,7 +9146,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="D53" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -9167,7 +9154,7 @@
         <v>676</v>
       </c>
       <c r="D60" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
   </sheetData>
@@ -9186,9 +9173,9 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76" bestFit="1" customWidth="1"/>
   </cols>
@@ -9333,7 +9320,7 @@
         <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -9344,7 +9331,7 @@
         <v>267</v>
       </c>
       <c r="D18" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -9352,7 +9339,7 @@
         <v>297</v>
       </c>
       <c r="D22" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -9385,18 +9372,18 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D31" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>761</v>
+      </c>
+      <c r="D32" t="s">
         <v>762</v>
-      </c>
-      <c r="D32" t="s">
-        <v>763</v>
       </c>
     </row>
   </sheetData>
@@ -9414,9 +9401,9 @@
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="94.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="94.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>